<commit_message>
detalles de ABM matricula y alumno
</commit_message>
<xml_diff>
--- a/procesos.xlsx
+++ b/procesos.xlsx
@@ -18,7 +18,6 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'1'!$10:$10</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -509,7 +508,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -710,6 +709,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -721,7 +723,70 @@
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5EBC78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDC913"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2575A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5EBC78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDC913"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2575A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5EBC78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDC913"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2575A"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1478,27 +1543,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5EBC78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDC913"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2575A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <bottom/>
         <horizontal style="thick">
@@ -1526,15 +1570,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Organizador de ideas" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="38"/>
-      <tableStyleElement type="headerRow" dxfId="37"/>
-      <tableStyleElement type="firstColumn" dxfId="36"/>
+      <tableStyleElement type="wholeTable" dxfId="44"/>
+      <tableStyleElement type="headerRow" dxfId="43"/>
+      <tableStyleElement type="firstColumn" dxfId="42"/>
     </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF5EBC78"/>
       <color rgb="FFF2575A"/>
-      <color rgb="FF5EBC78"/>
       <color rgb="FFFDC913"/>
       <color rgb="FFB64640"/>
       <color rgb="FF3F954D"/>
@@ -1601,7 +1645,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tareas" displayName="Tareas" ref="B10:G17" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tareas" displayName="Tareas" ref="B10:G17" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="B10:G17">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1611,14 +1655,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="6" name=" " dataDxfId="29"/>
-    <tableColumn id="1" name="Tareas" dataDxfId="28"/>
-    <tableColumn id="2" name="Fecha de vencimiento" dataDxfId="27"/>
-    <tableColumn id="3" name="¿Hecho?" dataDxfId="26"/>
-    <tableColumn id="4" name="Estado" dataDxfId="25">
+    <tableColumn id="6" name=" " dataDxfId="38"/>
+    <tableColumn id="1" name="Tareas" dataDxfId="37"/>
+    <tableColumn id="2" name="Fecha de vencimiento" dataDxfId="36"/>
+    <tableColumn id="3" name="¿Hecho?" dataDxfId="35"/>
+    <tableColumn id="4" name="Estado" dataDxfId="34">
       <calculatedColumnFormula>IF(Tareas[[#This Row],[¿Hecho?]]="SI",2,IF(Tareas[[#This Row],[¿Hecho?]]="no",0,IF(OR(AND(Tareas[[#This Row],[Fecha de vencimiento]]&lt;=TODAY(),Tareas[[#This Row],[Fecha de vencimiento]]&lt;FechaDeVencimiento),Tareas[[#This Row],[¿Hecho?]]="Pendiente"),1,"")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Notas" dataDxfId="24"/>
+    <tableColumn id="5" name="Notas" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="Organizador de ideas" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1630,17 +1674,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tareas9" displayName="Tareas9" ref="B10:G17" totalsRowShown="0" headerRowDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tareas9" displayName="Tareas9" ref="B10:G17" totalsRowShown="0" headerRowDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="B10:G17"/>
   <tableColumns count="6">
-    <tableColumn id="6" name=" " dataDxfId="17"/>
-    <tableColumn id="1" name="Tareas" dataDxfId="16"/>
-    <tableColumn id="2" name="Fecha de vencimiento" dataDxfId="15"/>
-    <tableColumn id="3" name="¿Hecho?" dataDxfId="14"/>
-    <tableColumn id="4" name="Estado" dataDxfId="13">
+    <tableColumn id="6" name=" " dataDxfId="26"/>
+    <tableColumn id="1" name="Tareas" dataDxfId="25"/>
+    <tableColumn id="2" name="Fecha de vencimiento" dataDxfId="24"/>
+    <tableColumn id="3" name="¿Hecho?" dataDxfId="23"/>
+    <tableColumn id="4" name="Estado" dataDxfId="22">
       <calculatedColumnFormula>IF(Tareas9[[#This Row],[¿Hecho?]]="SI",2,IF(Tareas9[[#This Row],[¿Hecho?]]="no",0,IF(OR(AND(Tareas9[[#This Row],[Fecha de vencimiento]]&lt;=TODAY(),Tareas9[[#This Row],[Fecha de vencimiento]]&lt;FechaDeVencimiento),Tareas9[[#This Row],[¿Hecho?]]="Pendiente"),1,"")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Notas" dataDxfId="12"/>
+    <tableColumn id="5" name="Notas" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="Organizador de ideas" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1652,17 +1696,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tareas911" displayName="Tareas911" ref="B10:G17" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tareas911" displayName="Tareas911" ref="B10:G17" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="B10:G17"/>
   <tableColumns count="6">
-    <tableColumn id="6" name=" " dataDxfId="5"/>
-    <tableColumn id="1" name="Tareas" dataDxfId="4"/>
-    <tableColumn id="2" name="Fecha de vencimiento" dataDxfId="3"/>
-    <tableColumn id="3" name="¿Hecho?" dataDxfId="2"/>
-    <tableColumn id="4" name="Estado" dataDxfId="1">
+    <tableColumn id="6" name=" " dataDxfId="14"/>
+    <tableColumn id="1" name="Tareas" dataDxfId="13"/>
+    <tableColumn id="2" name="Fecha de vencimiento" dataDxfId="12"/>
+    <tableColumn id="3" name="¿Hecho?" dataDxfId="11"/>
+    <tableColumn id="4" name="Estado" dataDxfId="10">
       <calculatedColumnFormula>IF(Tareas911[[#This Row],[¿Hecho?]]="SI",2,IF(Tareas911[[#This Row],[¿Hecho?]]="no",0,IF(OR(AND(Tareas911[[#This Row],[Fecha de vencimiento]]&lt;=TODAY(),Tareas911[[#This Row],[Fecha de vencimiento]]&lt;FechaDeVencimiento),Tareas911[[#This Row],[¿Hecho?]]="Pendiente"),1,"")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Notas" dataDxfId="0"/>
+    <tableColumn id="5" name="Notas" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Organizador de ideas" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1942,7 +1986,7 @@
   <dimension ref="A1:K154"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="D13:E13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="29.25" customHeight="1"/>
@@ -2111,7 +2155,7 @@
       <c r="G11" s="45"/>
     </row>
     <row r="12" spans="1:11" ht="33.75" customHeight="1">
-      <c r="B12" s="21">
+      <c r="B12" s="67">
         <v>2</v>
       </c>
       <c r="C12" s="30" t="s">
@@ -2121,11 +2165,11 @@
         <v>44722</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="32">
         <f ca="1">IF(Tareas[[#This Row],[¿Hecho?]]="SI",2,IF(Tareas[[#This Row],[¿Hecho?]]="no",0,IF(OR(AND(Tareas[[#This Row],[Fecha de vencimiento]]&lt;=TODAY(),Tareas[[#This Row],[Fecha de vencimiento]]&lt;FechaDeVencimiento),Tareas[[#This Row],[¿Hecho?]]="Pendiente"),1,"")))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="46" t="s">
         <v>29</v>
@@ -2142,11 +2186,11 @@
         <v>44722</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="33">
         <f ca="1">IF(Tareas[[#This Row],[¿Hecho?]]="SI",2,IF(Tareas[[#This Row],[¿Hecho?]]="no",0,IF(OR(AND(Tareas[[#This Row],[Fecha de vencimiento]]&lt;=TODAY(),Tareas[[#This Row],[Fecha de vencimiento]]&lt;FechaDeVencimiento),Tareas[[#This Row],[¿Hecho?]]="Pendiente"),1,"")))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="46" t="s">
         <v>30</v>
@@ -2163,11 +2207,11 @@
         <v>44722</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="32">
         <f ca="1">IF(Tareas[[#This Row],[¿Hecho?]]="SI",2,IF(Tareas[[#This Row],[¿Hecho?]]="no",0,IF(OR(AND(Tareas[[#This Row],[Fecha de vencimiento]]&lt;=TODAY(),Tareas[[#This Row],[Fecha de vencimiento]]&lt;FechaDeVencimiento),Tareas[[#This Row],[¿Hecho?]]="Pendiente"),1,"")))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="46" t="s">
         <v>28</v>
@@ -2184,11 +2228,11 @@
         <v>44722</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="37">
         <f ca="1">IF(Tareas[[#This Row],[¿Hecho?]]="SI",2,IF(Tareas[[#This Row],[¿Hecho?]]="no",0,IF(OR(AND(Tareas[[#This Row],[Fecha de vencimiento]]&lt;=TODAY(),Tareas[[#This Row],[Fecha de vencimiento]]&lt;FechaDeVencimiento),Tareas[[#This Row],[¿Hecho?]]="Pendiente"),1,"")))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="47" t="s">
         <v>27</v>
@@ -2205,11 +2249,11 @@
         <v>44722</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" s="37">
         <f ca="1">IF(Tareas[[#This Row],[¿Hecho?]]="SI",2,IF(Tareas[[#This Row],[¿Hecho?]]="no",0,IF(OR(AND(Tareas[[#This Row],[Fecha de vencimiento]]&lt;=TODAY(),Tareas[[#This Row],[Fecha de vencimiento]]&lt;FechaDeVencimiento),Tareas[[#This Row],[¿Hecho?]]="Pendiente"),1,"")))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="47" t="s">
         <v>26</v>
@@ -3340,18 +3384,18 @@
     <mergeCell ref="C6:C8"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B17">
-    <cfRule type="expression" dxfId="35" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$F11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$F11=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$F11=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F17">
-    <cfRule type="expression" dxfId="32" priority="25">
+    <cfRule type="expression" dxfId="41" priority="25">
       <formula>$F11&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4747,18 +4791,18 @@
     <mergeCell ref="D6:G8"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B17">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="32" priority="1">
       <formula>$F11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="2">
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>$F11=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="30" priority="3">
       <formula>$F11=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F17">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="29" priority="4">
       <formula>$F11&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6191,18 +6235,18 @@
     <mergeCell ref="D6:G8"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B17">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>$F11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$F11=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>$F11=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F17">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>$F11&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>